<commit_message>
1. Update script to support specify browser in the excel
2. Update script to add Skipped into result of final result if result column is blank

3. Update the script to support max size window, login and execute JavaScript in Firefox

4. Add Log method to output some logs to a log file of each Test case
</commit_message>
<xml_diff>
--- a/TestCaseData/Kerry_data_2c.xlsx
+++ b/TestCaseData/Kerry_data_2c.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="79">
   <si>
     <t>Case No</t>
   </si>
@@ -243,13 +243,22 @@
     <t>Sort Order3</t>
   </si>
   <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>Firefox</t>
+    <t>not yet</t>
   </si>
   <si>
     <t>aaa</t>
@@ -709,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -967,7 +976,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +996,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,7 +1036,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,7 +1056,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1067,7 +1076,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1093,7 +1102,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -2306,7 +2315,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>34</v>
@@ -2425,7 +2434,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="6" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>34</v>
@@ -2505,7 +2514,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>38</v>
@@ -2635,7 +2644,7 @@
   <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3809,7 +3818,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -3846,6 +3855,9 @@
       </c>
       <c r="D2" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>43</v>
@@ -3885,6 +3897,9 @@
       </c>
       <c r="D3" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>43</v>
@@ -3965,7 +3980,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5075,7 +5090,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -5112,8 +5127,11 @@
       <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="H2" s="6" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>34</v>
@@ -5151,8 +5169,11 @@
       <c r="D3" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="H3" s="6" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>34</v>
@@ -5230,7 +5251,7 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6532,7 +6553,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -6575,6 +6596,9 @@
       </c>
       <c r="D2" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>51</v>
@@ -6620,6 +6644,9 @@
       </c>
       <c r="D3" s="9" t="s">
         <v>17</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>43</v>
@@ -6706,7 +6733,7 @@
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8007,7 +8034,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -8055,7 +8082,9 @@
       <c r="D2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16" t="s">
+        <v>75</v>
+      </c>
       <c r="H2" s="6" t="s">
         <v>33</v>
       </c>
@@ -8098,7 +8127,9 @@
       <c r="D3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>74</v>
+      </c>
       <c r="H3" s="6" t="s">
         <v>43</v>
       </c>
@@ -8141,7 +8172,9 @@
       <c r="D4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="16"/>
+      <c r="E4" s="16" t="s">
+        <v>73</v>
+      </c>
       <c r="H4" s="6" t="s">
         <v>68</v>
       </c>
@@ -8202,7 +8235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -8993,7 +9026,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
TC1.py Add tag #@Begin and #@END to specify which part should be executed Framework.py Exchange to use TC_Runner to load the test cases TC_Runner.py Create to read the execute part by finding the tags and exec the part had success read Excel_x.py Update Select_Sheet_By_Name as openpyxl updated Report.py Add a executed colnum determine to ignore the bug when the executed colunm is null
</commit_message>
<xml_diff>
--- a/TestCaseData/Kerry_data_2c.xlsx
+++ b/TestCaseData/Kerry_data_2c.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="4" r:id="rId1"/>
@@ -12,16 +12,17 @@
     <sheet name="2" sheetId="6" r:id="rId3"/>
     <sheet name="3" sheetId="7" r:id="rId4"/>
     <sheet name="4" sheetId="8" r:id="rId5"/>
-    <sheet name="7" sheetId="11" r:id="rId6"/>
-    <sheet name="result-timestamp" sheetId="9" r:id="rId7"/>
-    <sheet name="data" sheetId="10" r:id="rId8"/>
+    <sheet name="6" sheetId="12" r:id="rId6"/>
+    <sheet name="7" sheetId="11" r:id="rId7"/>
+    <sheet name="result-timestamp" sheetId="9" r:id="rId8"/>
+    <sheet name="data" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="74">
   <si>
     <t>Case No</t>
   </si>
@@ -122,9 +123,6 @@
     <t>Assertion</t>
   </si>
   <si>
-    <t>Skip</t>
-  </si>
-  <si>
     <t>jack.li</t>
   </si>
   <si>
@@ -178,9 +176,6 @@
     <t>Phone Number</t>
   </si>
   <si>
-    <t>skip</t>
-  </si>
-  <si>
     <t>This field is required</t>
   </si>
   <si>
@@ -231,9 +226,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>Skipped</t>
-  </si>
-  <si>
     <t>Sort Order1</t>
   </si>
   <si>
@@ -246,13 +238,7 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>IE</t>
-  </si>
-  <si>
     <t>Firefox</t>
-  </si>
-  <si>
-    <t>Chrome</t>
   </si>
   <si>
     <t>no</t>
@@ -261,7 +247,7 @@
     <t>not yet</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>IE</t>
   </si>
 </sst>
 </file>
@@ -719,7 +705,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -976,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -996,7 +982,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,7 +1002,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1036,7 +1022,7 @@
         <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1053,10 +1039,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,7 +1050,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
@@ -1076,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,7 +1088,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2276,7 +2262,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -2314,17 +2300,20 @@
       <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="H2" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -2353,17 +2342,18 @@
       <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="E3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="6"/>
       <c r="J3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -2392,17 +2382,18 @@
       <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="E4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="6"/>
       <c r="J4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -2431,19 +2422,20 @@
       <c r="D5" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="E5" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
-      <c r="H5" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="H5" s="6"/>
       <c r="J5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -2472,19 +2464,20 @@
       <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="E6" s="9" t="s">
+        <v>73</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
-      <c r="H6" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="H6" s="6"/>
       <c r="J6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="K6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -2516,17 +2509,15 @@
       <c r="E7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="6"/>
+      <c r="J7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="K7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="L7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -2542,17 +2533,18 @@
       <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="E8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="6"/>
+      <c r="J8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -2568,17 +2560,18 @@
       <c r="D9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="E9" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="J9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="K9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -2594,17 +2587,18 @@
       <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="E10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="6"/>
       <c r="J10" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -2620,17 +2614,18 @@
       <c r="D11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="E11" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="J11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2644,7 +2639,7 @@
   <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3809,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -3818,7 +3813,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -3857,19 +3852,19 @@
         <v>12</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
@@ -3899,19 +3894,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
@@ -3980,7 +3975,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5090,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -5128,19 +5123,19 @@
         <v>12</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S2" s="10"/>
       <c r="T2" s="10"/>
@@ -5170,19 +5165,19 @@
         <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -5251,7 +5246,7 @@
   <dimension ref="A1:AH5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6541,7 +6536,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>26</v>
@@ -6553,7 +6548,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -6574,10 +6569,10 @@
         <v>32</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
@@ -6598,25 +6593,25 @@
         <v>17</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="V2" s="10"/>
       <c r="W2" s="12"/>
@@ -6646,25 +6641,25 @@
         <v>17</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="L3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
@@ -6733,7 +6728,7 @@
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8022,7 +8017,7 @@
   <sheetData>
     <row r="1" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>26</v>
@@ -8034,7 +8029,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>27</v>
@@ -8055,16 +8050,16 @@
         <v>32</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
@@ -8077,28 +8072,28 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U2" s="10"/>
       <c r="V2" s="12"/>
@@ -8128,22 +8123,20 @@
         <v>20</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="H3" s="6"/>
       <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="L3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
@@ -8173,22 +8166,20 @@
         <v>20</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>68</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="H4" s="6"/>
       <c r="J4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="L4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
@@ -8232,6 +8223,1505 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG5"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" style="6" customWidth="1"/>
+    <col min="16" max="26" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="33" width="20" style="6" customWidth="1"/>
+    <col min="34" max="34" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.140625" style="6" customWidth="1"/>
+    <col min="36" max="256" width="22.140625" style="6"/>
+    <col min="257" max="257" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="16.85546875" style="6" customWidth="1"/>
+    <col min="265" max="265" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="27.7109375" style="6" customWidth="1"/>
+    <col min="272" max="282" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="283" max="289" width="20" style="6" customWidth="1"/>
+    <col min="290" max="290" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="22.140625" style="6" customWidth="1"/>
+    <col min="292" max="512" width="22.140625" style="6"/>
+    <col min="513" max="513" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="516" max="516" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="517" max="517" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="518" max="518" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="519" max="519" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="16.85546875" style="6" customWidth="1"/>
+    <col min="521" max="521" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="524" max="524" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="525" max="525" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="526" max="526" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="27.7109375" style="6" customWidth="1"/>
+    <col min="528" max="538" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="539" max="545" width="20" style="6" customWidth="1"/>
+    <col min="546" max="546" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="547" max="547" width="22.140625" style="6" customWidth="1"/>
+    <col min="548" max="768" width="22.140625" style="6"/>
+    <col min="769" max="769" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="772" max="772" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="773" max="773" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="774" max="774" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="775" max="775" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="16.85546875" style="6" customWidth="1"/>
+    <col min="777" max="777" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="778" max="778" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="779" max="779" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="780" max="780" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="781" max="781" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="782" max="782" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="783" max="783" width="27.7109375" style="6" customWidth="1"/>
+    <col min="784" max="794" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="795" max="801" width="20" style="6" customWidth="1"/>
+    <col min="802" max="802" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="803" max="803" width="22.140625" style="6" customWidth="1"/>
+    <col min="804" max="1024" width="22.140625" style="6"/>
+    <col min="1025" max="1025" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1028" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1029" max="1029" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1030" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1031" max="1031" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="16.85546875" style="6" customWidth="1"/>
+    <col min="1033" max="1033" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1034" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1035" max="1035" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1036" max="1036" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1037" max="1037" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1038" max="1038" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1039" width="27.7109375" style="6" customWidth="1"/>
+    <col min="1040" max="1050" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="1051" max="1057" width="20" style="6" customWidth="1"/>
+    <col min="1058" max="1058" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="1059" max="1059" width="22.140625" style="6" customWidth="1"/>
+    <col min="1060" max="1280" width="22.140625" style="6"/>
+    <col min="1281" max="1281" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1284" max="1284" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1285" max="1285" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1286" max="1286" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1287" max="1287" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="16.85546875" style="6" customWidth="1"/>
+    <col min="1289" max="1289" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1290" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1291" max="1291" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1292" max="1292" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1293" max="1293" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1294" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1295" width="27.7109375" style="6" customWidth="1"/>
+    <col min="1296" max="1306" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="1307" max="1313" width="20" style="6" customWidth="1"/>
+    <col min="1314" max="1314" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="1315" max="1315" width="22.140625" style="6" customWidth="1"/>
+    <col min="1316" max="1536" width="22.140625" style="6"/>
+    <col min="1537" max="1537" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1540" max="1540" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1541" max="1541" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1542" max="1542" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1543" max="1543" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="16.85546875" style="6" customWidth="1"/>
+    <col min="1545" max="1545" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1546" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1547" max="1547" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1548" max="1548" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1549" max="1549" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1550" max="1550" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1551" width="27.7109375" style="6" customWidth="1"/>
+    <col min="1552" max="1562" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="1563" max="1569" width="20" style="6" customWidth="1"/>
+    <col min="1570" max="1570" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="1571" max="1571" width="22.140625" style="6" customWidth="1"/>
+    <col min="1572" max="1792" width="22.140625" style="6"/>
+    <col min="1793" max="1793" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1796" max="1796" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1797" max="1797" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1798" max="1798" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1799" max="1799" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="16.85546875" style="6" customWidth="1"/>
+    <col min="1801" max="1801" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1802" max="1802" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1803" max="1803" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1804" max="1804" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1805" max="1805" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1806" max="1806" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1807" max="1807" width="27.7109375" style="6" customWidth="1"/>
+    <col min="1808" max="1818" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="1819" max="1825" width="20" style="6" customWidth="1"/>
+    <col min="1826" max="1826" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="1827" max="1827" width="22.140625" style="6" customWidth="1"/>
+    <col min="1828" max="2048" width="22.140625" style="6"/>
+    <col min="2049" max="2049" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2052" max="2052" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2053" max="2053" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2054" max="2054" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2055" max="2055" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="16.85546875" style="6" customWidth="1"/>
+    <col min="2057" max="2057" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2058" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2059" max="2059" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2060" max="2060" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2061" max="2061" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2062" max="2062" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2063" width="27.7109375" style="6" customWidth="1"/>
+    <col min="2064" max="2074" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="2075" max="2081" width="20" style="6" customWidth="1"/>
+    <col min="2082" max="2082" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2083" max="2083" width="22.140625" style="6" customWidth="1"/>
+    <col min="2084" max="2304" width="22.140625" style="6"/>
+    <col min="2305" max="2305" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2308" max="2308" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2309" max="2309" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2310" max="2310" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2311" max="2311" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="16.85546875" style="6" customWidth="1"/>
+    <col min="2313" max="2313" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2314" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2315" max="2315" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2316" max="2316" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2317" max="2317" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2318" max="2318" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2319" width="27.7109375" style="6" customWidth="1"/>
+    <col min="2320" max="2330" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="2331" max="2337" width="20" style="6" customWidth="1"/>
+    <col min="2338" max="2338" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2339" max="2339" width="22.140625" style="6" customWidth="1"/>
+    <col min="2340" max="2560" width="22.140625" style="6"/>
+    <col min="2561" max="2561" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2564" max="2564" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2565" max="2565" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2566" max="2566" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2567" max="2567" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="16.85546875" style="6" customWidth="1"/>
+    <col min="2569" max="2569" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2570" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2571" max="2571" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2572" max="2572" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2573" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2574" max="2574" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2575" width="27.7109375" style="6" customWidth="1"/>
+    <col min="2576" max="2586" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="2587" max="2593" width="20" style="6" customWidth="1"/>
+    <col min="2594" max="2594" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2595" max="2595" width="22.140625" style="6" customWidth="1"/>
+    <col min="2596" max="2816" width="22.140625" style="6"/>
+    <col min="2817" max="2817" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2820" max="2820" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2821" max="2821" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2822" max="2822" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2823" max="2823" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="16.85546875" style="6" customWidth="1"/>
+    <col min="2825" max="2825" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2826" max="2826" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2827" max="2827" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2828" max="2828" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2829" max="2829" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2830" max="2830" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2831" max="2831" width="27.7109375" style="6" customWidth="1"/>
+    <col min="2832" max="2842" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="2843" max="2849" width="20" style="6" customWidth="1"/>
+    <col min="2850" max="2850" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="2851" max="2851" width="22.140625" style="6" customWidth="1"/>
+    <col min="2852" max="3072" width="22.140625" style="6"/>
+    <col min="3073" max="3073" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3076" max="3076" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3077" max="3077" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3078" max="3078" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3079" max="3079" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="16.85546875" style="6" customWidth="1"/>
+    <col min="3081" max="3081" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3082" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3083" max="3083" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3084" max="3084" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3085" max="3085" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3086" max="3086" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3087" width="27.7109375" style="6" customWidth="1"/>
+    <col min="3088" max="3098" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="3099" max="3105" width="20" style="6" customWidth="1"/>
+    <col min="3106" max="3106" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="3107" max="3107" width="22.140625" style="6" customWidth="1"/>
+    <col min="3108" max="3328" width="22.140625" style="6"/>
+    <col min="3329" max="3329" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3332" max="3332" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3333" max="3333" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3334" max="3334" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3335" max="3335" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="16.85546875" style="6" customWidth="1"/>
+    <col min="3337" max="3337" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3338" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3339" max="3339" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3340" max="3340" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3341" max="3341" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3342" max="3342" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3343" width="27.7109375" style="6" customWidth="1"/>
+    <col min="3344" max="3354" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="3355" max="3361" width="20" style="6" customWidth="1"/>
+    <col min="3362" max="3362" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="3363" max="3363" width="22.140625" style="6" customWidth="1"/>
+    <col min="3364" max="3584" width="22.140625" style="6"/>
+    <col min="3585" max="3585" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3588" max="3588" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3589" max="3589" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3590" max="3590" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3591" max="3591" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="16.85546875" style="6" customWidth="1"/>
+    <col min="3593" max="3593" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3594" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3595" max="3595" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3596" max="3596" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3597" max="3597" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3598" max="3598" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3599" width="27.7109375" style="6" customWidth="1"/>
+    <col min="3600" max="3610" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="3611" max="3617" width="20" style="6" customWidth="1"/>
+    <col min="3618" max="3618" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="3619" max="3619" width="22.140625" style="6" customWidth="1"/>
+    <col min="3620" max="3840" width="22.140625" style="6"/>
+    <col min="3841" max="3841" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3844" max="3844" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3845" max="3845" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3846" max="3846" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3847" max="3847" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="16.85546875" style="6" customWidth="1"/>
+    <col min="3849" max="3849" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3850" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3851" max="3851" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3852" max="3852" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3853" max="3853" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3854" max="3854" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3855" max="3855" width="27.7109375" style="6" customWidth="1"/>
+    <col min="3856" max="3866" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="3867" max="3873" width="20" style="6" customWidth="1"/>
+    <col min="3874" max="3874" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="3875" max="3875" width="22.140625" style="6" customWidth="1"/>
+    <col min="3876" max="4096" width="22.140625" style="6"/>
+    <col min="4097" max="4097" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4100" max="4100" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4101" max="4101" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4102" max="4102" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4103" max="4103" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="16.85546875" style="6" customWidth="1"/>
+    <col min="4105" max="4105" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4106" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4107" max="4107" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4108" max="4108" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4109" max="4109" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4110" max="4110" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4111" width="27.7109375" style="6" customWidth="1"/>
+    <col min="4112" max="4122" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="4123" max="4129" width="20" style="6" customWidth="1"/>
+    <col min="4130" max="4130" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="4131" max="4131" width="22.140625" style="6" customWidth="1"/>
+    <col min="4132" max="4352" width="22.140625" style="6"/>
+    <col min="4353" max="4353" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4356" max="4356" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4357" max="4357" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4358" max="4358" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4359" max="4359" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="16.85546875" style="6" customWidth="1"/>
+    <col min="4361" max="4361" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4362" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4363" max="4363" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4364" max="4364" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4365" max="4365" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4366" max="4366" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4367" width="27.7109375" style="6" customWidth="1"/>
+    <col min="4368" max="4378" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="4379" max="4385" width="20" style="6" customWidth="1"/>
+    <col min="4386" max="4386" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="4387" max="4387" width="22.140625" style="6" customWidth="1"/>
+    <col min="4388" max="4608" width="22.140625" style="6"/>
+    <col min="4609" max="4609" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4612" max="4612" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4613" max="4613" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4614" max="4614" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4615" max="4615" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="16.85546875" style="6" customWidth="1"/>
+    <col min="4617" max="4617" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4618" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4619" max="4619" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4620" max="4620" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4621" max="4621" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4622" max="4622" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4623" width="27.7109375" style="6" customWidth="1"/>
+    <col min="4624" max="4634" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="4635" max="4641" width="20" style="6" customWidth="1"/>
+    <col min="4642" max="4642" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="4643" max="4643" width="22.140625" style="6" customWidth="1"/>
+    <col min="4644" max="4864" width="22.140625" style="6"/>
+    <col min="4865" max="4865" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4868" max="4868" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4869" max="4869" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4870" max="4870" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4871" max="4871" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="16.85546875" style="6" customWidth="1"/>
+    <col min="4873" max="4873" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4874" max="4874" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4875" max="4875" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4876" max="4876" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4877" max="4877" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4878" max="4878" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4879" max="4879" width="27.7109375" style="6" customWidth="1"/>
+    <col min="4880" max="4890" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="4891" max="4897" width="20" style="6" customWidth="1"/>
+    <col min="4898" max="4898" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="4899" max="4899" width="22.140625" style="6" customWidth="1"/>
+    <col min="4900" max="5120" width="22.140625" style="6"/>
+    <col min="5121" max="5121" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5124" max="5124" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5125" max="5125" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5126" max="5126" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5127" max="5127" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="16.85546875" style="6" customWidth="1"/>
+    <col min="5129" max="5129" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5130" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5131" max="5131" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5132" max="5132" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5133" max="5133" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5134" max="5134" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5135" width="27.7109375" style="6" customWidth="1"/>
+    <col min="5136" max="5146" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="5147" max="5153" width="20" style="6" customWidth="1"/>
+    <col min="5154" max="5154" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="5155" max="5155" width="22.140625" style="6" customWidth="1"/>
+    <col min="5156" max="5376" width="22.140625" style="6"/>
+    <col min="5377" max="5377" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5380" max="5380" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5381" max="5381" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5382" max="5382" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5383" max="5383" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="16.85546875" style="6" customWidth="1"/>
+    <col min="5385" max="5385" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5386" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5387" max="5387" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5388" max="5388" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5389" max="5389" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5390" max="5390" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5391" width="27.7109375" style="6" customWidth="1"/>
+    <col min="5392" max="5402" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="5403" max="5409" width="20" style="6" customWidth="1"/>
+    <col min="5410" max="5410" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="5411" max="5411" width="22.140625" style="6" customWidth="1"/>
+    <col min="5412" max="5632" width="22.140625" style="6"/>
+    <col min="5633" max="5633" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5636" max="5636" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5637" max="5637" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5638" max="5638" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5639" max="5639" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="16.85546875" style="6" customWidth="1"/>
+    <col min="5641" max="5641" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5642" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5643" max="5643" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5644" max="5644" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5645" max="5645" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5646" max="5646" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5647" width="27.7109375" style="6" customWidth="1"/>
+    <col min="5648" max="5658" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="5659" max="5665" width="20" style="6" customWidth="1"/>
+    <col min="5666" max="5666" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="5667" max="5667" width="22.140625" style="6" customWidth="1"/>
+    <col min="5668" max="5888" width="22.140625" style="6"/>
+    <col min="5889" max="5889" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5892" max="5892" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5893" max="5893" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5894" max="5894" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5895" max="5895" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="16.85546875" style="6" customWidth="1"/>
+    <col min="5897" max="5897" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5898" max="5898" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5899" max="5899" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5900" max="5900" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5901" max="5901" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5902" max="5902" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5903" max="5903" width="27.7109375" style="6" customWidth="1"/>
+    <col min="5904" max="5914" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="5915" max="5921" width="20" style="6" customWidth="1"/>
+    <col min="5922" max="5922" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="5923" max="5923" width="22.140625" style="6" customWidth="1"/>
+    <col min="5924" max="6144" width="22.140625" style="6"/>
+    <col min="6145" max="6145" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6148" max="6148" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6149" max="6149" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6150" max="6150" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6151" max="6151" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="16.85546875" style="6" customWidth="1"/>
+    <col min="6153" max="6153" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6154" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6155" max="6155" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6156" max="6156" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6157" max="6157" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6158" max="6158" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6159" width="27.7109375" style="6" customWidth="1"/>
+    <col min="6160" max="6170" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="6171" max="6177" width="20" style="6" customWidth="1"/>
+    <col min="6178" max="6178" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="6179" max="6179" width="22.140625" style="6" customWidth="1"/>
+    <col min="6180" max="6400" width="22.140625" style="6"/>
+    <col min="6401" max="6401" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6404" max="6404" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6405" max="6405" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6406" max="6406" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6407" max="6407" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="16.85546875" style="6" customWidth="1"/>
+    <col min="6409" max="6409" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6410" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6411" max="6411" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6412" max="6412" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6413" max="6413" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6414" max="6414" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6415" width="27.7109375" style="6" customWidth="1"/>
+    <col min="6416" max="6426" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="6427" max="6433" width="20" style="6" customWidth="1"/>
+    <col min="6434" max="6434" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="6435" max="6435" width="22.140625" style="6" customWidth="1"/>
+    <col min="6436" max="6656" width="22.140625" style="6"/>
+    <col min="6657" max="6657" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6660" max="6660" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6661" max="6661" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6662" max="6662" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6663" max="6663" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="16.85546875" style="6" customWidth="1"/>
+    <col min="6665" max="6665" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6666" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6667" max="6667" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6668" max="6668" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6669" max="6669" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6670" max="6670" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6671" width="27.7109375" style="6" customWidth="1"/>
+    <col min="6672" max="6682" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="6683" max="6689" width="20" style="6" customWidth="1"/>
+    <col min="6690" max="6690" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="6691" max="6691" width="22.140625" style="6" customWidth="1"/>
+    <col min="6692" max="6912" width="22.140625" style="6"/>
+    <col min="6913" max="6913" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6916" max="6916" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6917" max="6917" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6918" max="6918" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6919" max="6919" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="16.85546875" style="6" customWidth="1"/>
+    <col min="6921" max="6921" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6922" max="6922" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6923" max="6923" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6924" max="6924" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6925" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6926" max="6926" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="6927" max="6927" width="27.7109375" style="6" customWidth="1"/>
+    <col min="6928" max="6938" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="6939" max="6945" width="20" style="6" customWidth="1"/>
+    <col min="6946" max="6946" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="6947" max="6947" width="22.140625" style="6" customWidth="1"/>
+    <col min="6948" max="7168" width="22.140625" style="6"/>
+    <col min="7169" max="7169" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7172" max="7172" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7173" max="7173" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7174" max="7174" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7175" max="7175" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="16.85546875" style="6" customWidth="1"/>
+    <col min="7177" max="7177" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7178" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7179" max="7179" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7180" max="7180" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7181" max="7181" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7182" max="7182" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7183" width="27.7109375" style="6" customWidth="1"/>
+    <col min="7184" max="7194" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="7195" max="7201" width="20" style="6" customWidth="1"/>
+    <col min="7202" max="7202" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="7203" max="7203" width="22.140625" style="6" customWidth="1"/>
+    <col min="7204" max="7424" width="22.140625" style="6"/>
+    <col min="7425" max="7425" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7428" max="7428" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7429" max="7429" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7430" max="7430" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7431" max="7431" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="16.85546875" style="6" customWidth="1"/>
+    <col min="7433" max="7433" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7434" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7435" max="7435" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7436" max="7436" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7437" max="7437" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7438" max="7438" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7439" width="27.7109375" style="6" customWidth="1"/>
+    <col min="7440" max="7450" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="7451" max="7457" width="20" style="6" customWidth="1"/>
+    <col min="7458" max="7458" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="7459" max="7459" width="22.140625" style="6" customWidth="1"/>
+    <col min="7460" max="7680" width="22.140625" style="6"/>
+    <col min="7681" max="7681" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7684" max="7684" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7685" max="7685" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7686" max="7686" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7687" max="7687" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="16.85546875" style="6" customWidth="1"/>
+    <col min="7689" max="7689" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7690" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7691" max="7691" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7692" max="7692" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7693" max="7693" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7694" max="7694" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7695" width="27.7109375" style="6" customWidth="1"/>
+    <col min="7696" max="7706" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="7707" max="7713" width="20" style="6" customWidth="1"/>
+    <col min="7714" max="7714" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="7715" max="7715" width="22.140625" style="6" customWidth="1"/>
+    <col min="7716" max="7936" width="22.140625" style="6"/>
+    <col min="7937" max="7937" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7940" max="7940" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7941" max="7941" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7942" max="7942" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7943" max="7943" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="16.85546875" style="6" customWidth="1"/>
+    <col min="7945" max="7945" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7946" max="7946" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7947" max="7947" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7948" max="7948" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7949" max="7949" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7950" max="7950" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7951" max="7951" width="27.7109375" style="6" customWidth="1"/>
+    <col min="7952" max="7962" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="7963" max="7969" width="20" style="6" customWidth="1"/>
+    <col min="7970" max="7970" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="7971" max="7971" width="22.140625" style="6" customWidth="1"/>
+    <col min="7972" max="8192" width="22.140625" style="6"/>
+    <col min="8193" max="8193" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8196" max="8196" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8197" max="8197" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8198" max="8198" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8199" max="8199" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="16.85546875" style="6" customWidth="1"/>
+    <col min="8201" max="8201" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8202" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8203" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8204" max="8204" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8205" max="8205" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8206" max="8206" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8207" width="27.7109375" style="6" customWidth="1"/>
+    <col min="8208" max="8218" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="8219" max="8225" width="20" style="6" customWidth="1"/>
+    <col min="8226" max="8226" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8227" max="8227" width="22.140625" style="6" customWidth="1"/>
+    <col min="8228" max="8448" width="22.140625" style="6"/>
+    <col min="8449" max="8449" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8452" max="8452" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8453" max="8453" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8454" max="8454" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8455" max="8455" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="16.85546875" style="6" customWidth="1"/>
+    <col min="8457" max="8457" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8458" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8459" max="8459" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8460" max="8460" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8461" max="8461" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8462" max="8462" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8463" width="27.7109375" style="6" customWidth="1"/>
+    <col min="8464" max="8474" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="8475" max="8481" width="20" style="6" customWidth="1"/>
+    <col min="8482" max="8482" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8483" max="8483" width="22.140625" style="6" customWidth="1"/>
+    <col min="8484" max="8704" width="22.140625" style="6"/>
+    <col min="8705" max="8705" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8708" max="8708" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8709" max="8709" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8710" max="8710" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8711" max="8711" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="16.85546875" style="6" customWidth="1"/>
+    <col min="8713" max="8713" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8714" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8715" max="8715" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8716" max="8716" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8717" max="8717" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8718" max="8718" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8719" width="27.7109375" style="6" customWidth="1"/>
+    <col min="8720" max="8730" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="8731" max="8737" width="20" style="6" customWidth="1"/>
+    <col min="8738" max="8738" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8739" max="8739" width="22.140625" style="6" customWidth="1"/>
+    <col min="8740" max="8960" width="22.140625" style="6"/>
+    <col min="8961" max="8961" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8964" max="8964" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8965" max="8965" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8966" max="8966" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8967" max="8967" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="16.85546875" style="6" customWidth="1"/>
+    <col min="8969" max="8969" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8970" max="8970" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8971" max="8971" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8972" max="8972" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8973" max="8973" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8974" max="8974" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8975" max="8975" width="27.7109375" style="6" customWidth="1"/>
+    <col min="8976" max="8986" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="8987" max="8993" width="20" style="6" customWidth="1"/>
+    <col min="8994" max="8994" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="8995" max="8995" width="22.140625" style="6" customWidth="1"/>
+    <col min="8996" max="9216" width="22.140625" style="6"/>
+    <col min="9217" max="9217" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9220" max="9220" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9221" max="9221" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9222" max="9222" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9223" max="9223" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="16.85546875" style="6" customWidth="1"/>
+    <col min="9225" max="9225" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9226" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9227" max="9227" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9228" max="9228" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9229" max="9229" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9230" max="9230" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9231" width="27.7109375" style="6" customWidth="1"/>
+    <col min="9232" max="9242" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="9243" max="9249" width="20" style="6" customWidth="1"/>
+    <col min="9250" max="9250" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="9251" max="9251" width="22.140625" style="6" customWidth="1"/>
+    <col min="9252" max="9472" width="22.140625" style="6"/>
+    <col min="9473" max="9473" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9476" max="9476" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9477" max="9477" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9478" max="9478" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9479" max="9479" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="16.85546875" style="6" customWidth="1"/>
+    <col min="9481" max="9481" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9482" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9483" max="9483" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9484" max="9484" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9485" max="9485" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9486" max="9486" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9487" width="27.7109375" style="6" customWidth="1"/>
+    <col min="9488" max="9498" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="9499" max="9505" width="20" style="6" customWidth="1"/>
+    <col min="9506" max="9506" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="9507" max="9507" width="22.140625" style="6" customWidth="1"/>
+    <col min="9508" max="9728" width="22.140625" style="6"/>
+    <col min="9729" max="9729" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9732" max="9732" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9733" max="9733" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9734" max="9734" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9735" max="9735" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="16.85546875" style="6" customWidth="1"/>
+    <col min="9737" max="9737" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9738" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9739" max="9739" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9740" max="9740" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9741" max="9741" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9742" max="9742" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9743" width="27.7109375" style="6" customWidth="1"/>
+    <col min="9744" max="9754" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="9755" max="9761" width="20" style="6" customWidth="1"/>
+    <col min="9762" max="9762" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="9763" max="9763" width="22.140625" style="6" customWidth="1"/>
+    <col min="9764" max="9984" width="22.140625" style="6"/>
+    <col min="9985" max="9985" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9988" max="9988" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9989" max="9989" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9990" max="9990" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9991" max="9991" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="16.85546875" style="6" customWidth="1"/>
+    <col min="9993" max="9993" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9994" max="9994" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9995" max="9995" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9996" max="9996" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9997" max="9997" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9998" max="9998" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9999" max="9999" width="27.7109375" style="6" customWidth="1"/>
+    <col min="10000" max="10010" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="10011" max="10017" width="20" style="6" customWidth="1"/>
+    <col min="10018" max="10018" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="10019" max="10019" width="22.140625" style="6" customWidth="1"/>
+    <col min="10020" max="10240" width="22.140625" style="6"/>
+    <col min="10241" max="10241" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10244" max="10244" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10245" max="10245" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10246" max="10246" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10247" max="10247" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10249" max="10249" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10250" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10251" max="10251" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10252" max="10252" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10253" max="10253" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10254" max="10254" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10255" width="27.7109375" style="6" customWidth="1"/>
+    <col min="10256" max="10266" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="10267" max="10273" width="20" style="6" customWidth="1"/>
+    <col min="10274" max="10274" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="10275" max="10275" width="22.140625" style="6" customWidth="1"/>
+    <col min="10276" max="10496" width="22.140625" style="6"/>
+    <col min="10497" max="10497" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10500" max="10500" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10501" max="10501" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10502" max="10502" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10503" max="10503" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10505" max="10505" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10506" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10507" max="10507" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10508" max="10508" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10509" max="10509" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10510" max="10510" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10511" width="27.7109375" style="6" customWidth="1"/>
+    <col min="10512" max="10522" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="10523" max="10529" width="20" style="6" customWidth="1"/>
+    <col min="10530" max="10530" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="10531" max="10531" width="22.140625" style="6" customWidth="1"/>
+    <col min="10532" max="10752" width="22.140625" style="6"/>
+    <col min="10753" max="10753" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10756" max="10756" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10757" max="10757" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10758" max="10758" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10759" max="10759" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="16.85546875" style="6" customWidth="1"/>
+    <col min="10761" max="10761" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10762" max="10762" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10763" max="10763" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10764" max="10764" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10765" max="10765" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10766" max="10766" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10767" max="10767" width="27.7109375" style="6" customWidth="1"/>
+    <col min="10768" max="10778" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="10779" max="10785" width="20" style="6" customWidth="1"/>
+    <col min="10786" max="10786" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="10787" max="10787" width="22.140625" style="6" customWidth="1"/>
+    <col min="10788" max="11008" width="22.140625" style="6"/>
+    <col min="11009" max="11009" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11012" max="11012" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11013" max="11013" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11014" max="11014" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11015" max="11015" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="16.85546875" style="6" customWidth="1"/>
+    <col min="11017" max="11017" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11018" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11019" max="11019" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11020" max="11020" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11021" max="11021" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11022" max="11022" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11023" width="27.7109375" style="6" customWidth="1"/>
+    <col min="11024" max="11034" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="11035" max="11041" width="20" style="6" customWidth="1"/>
+    <col min="11042" max="11042" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="11043" max="11043" width="22.140625" style="6" customWidth="1"/>
+    <col min="11044" max="11264" width="22.140625" style="6"/>
+    <col min="11265" max="11265" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11268" max="11268" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11269" max="11269" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11270" max="11270" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11271" max="11271" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="16.85546875" style="6" customWidth="1"/>
+    <col min="11273" max="11273" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11274" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11275" max="11275" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11276" max="11276" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11277" max="11277" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11278" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11279" width="27.7109375" style="6" customWidth="1"/>
+    <col min="11280" max="11290" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="11291" max="11297" width="20" style="6" customWidth="1"/>
+    <col min="11298" max="11298" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="11299" max="11299" width="22.140625" style="6" customWidth="1"/>
+    <col min="11300" max="11520" width="22.140625" style="6"/>
+    <col min="11521" max="11521" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11524" max="11524" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11525" max="11525" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11526" max="11526" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11527" max="11527" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="16.85546875" style="6" customWidth="1"/>
+    <col min="11529" max="11529" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11530" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11531" max="11531" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11532" max="11532" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11533" max="11533" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11534" max="11534" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11535" width="27.7109375" style="6" customWidth="1"/>
+    <col min="11536" max="11546" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="11547" max="11553" width="20" style="6" customWidth="1"/>
+    <col min="11554" max="11554" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="11555" max="11555" width="22.140625" style="6" customWidth="1"/>
+    <col min="11556" max="11776" width="22.140625" style="6"/>
+    <col min="11777" max="11777" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11780" max="11780" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11781" max="11781" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11782" max="11782" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11783" max="11783" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="16.85546875" style="6" customWidth="1"/>
+    <col min="11785" max="11785" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="11786" max="11786" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11787" max="11787" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11788" max="11788" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11789" max="11789" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11790" max="11790" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11791" max="11791" width="27.7109375" style="6" customWidth="1"/>
+    <col min="11792" max="11802" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="11803" max="11809" width="20" style="6" customWidth="1"/>
+    <col min="11810" max="11810" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="11811" max="11811" width="22.140625" style="6" customWidth="1"/>
+    <col min="11812" max="12032" width="22.140625" style="6"/>
+    <col min="12033" max="12033" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12036" max="12036" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12037" max="12037" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12038" max="12038" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12039" max="12039" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="16.85546875" style="6" customWidth="1"/>
+    <col min="12041" max="12041" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12042" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12043" max="12043" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12044" max="12044" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12045" max="12045" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12046" max="12046" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12047" width="27.7109375" style="6" customWidth="1"/>
+    <col min="12048" max="12058" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="12059" max="12065" width="20" style="6" customWidth="1"/>
+    <col min="12066" max="12066" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="12067" max="12067" width="22.140625" style="6" customWidth="1"/>
+    <col min="12068" max="12288" width="22.140625" style="6"/>
+    <col min="12289" max="12289" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12292" max="12292" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12293" max="12293" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12294" max="12294" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12295" max="12295" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="16.85546875" style="6" customWidth="1"/>
+    <col min="12297" max="12297" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12298" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12299" max="12299" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12300" max="12300" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12301" max="12301" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12302" max="12302" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12303" width="27.7109375" style="6" customWidth="1"/>
+    <col min="12304" max="12314" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="12315" max="12321" width="20" style="6" customWidth="1"/>
+    <col min="12322" max="12322" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="12323" max="12323" width="22.140625" style="6" customWidth="1"/>
+    <col min="12324" max="12544" width="22.140625" style="6"/>
+    <col min="12545" max="12545" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12548" max="12548" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12549" max="12549" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12550" max="12550" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12551" max="12551" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="16.85546875" style="6" customWidth="1"/>
+    <col min="12553" max="12553" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12554" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12555" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12556" max="12556" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12557" max="12557" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12558" max="12558" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12559" width="27.7109375" style="6" customWidth="1"/>
+    <col min="12560" max="12570" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="12571" max="12577" width="20" style="6" customWidth="1"/>
+    <col min="12578" max="12578" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="12579" max="12579" width="22.140625" style="6" customWidth="1"/>
+    <col min="12580" max="12800" width="22.140625" style="6"/>
+    <col min="12801" max="12801" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12804" max="12804" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12805" max="12805" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12806" max="12806" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12807" max="12807" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="16.85546875" style="6" customWidth="1"/>
+    <col min="12809" max="12809" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12810" max="12810" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12811" max="12811" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12812" max="12812" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12813" max="12813" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12814" max="12814" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="12815" max="12815" width="27.7109375" style="6" customWidth="1"/>
+    <col min="12816" max="12826" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="12827" max="12833" width="20" style="6" customWidth="1"/>
+    <col min="12834" max="12834" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="12835" max="12835" width="22.140625" style="6" customWidth="1"/>
+    <col min="12836" max="13056" width="22.140625" style="6"/>
+    <col min="13057" max="13057" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13060" max="13060" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13061" max="13061" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13062" max="13062" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13063" max="13063" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="16.85546875" style="6" customWidth="1"/>
+    <col min="13065" max="13065" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13066" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13067" max="13067" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13068" max="13068" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13069" max="13069" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13070" max="13070" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13071" width="27.7109375" style="6" customWidth="1"/>
+    <col min="13072" max="13082" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="13083" max="13089" width="20" style="6" customWidth="1"/>
+    <col min="13090" max="13090" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="13091" max="13091" width="22.140625" style="6" customWidth="1"/>
+    <col min="13092" max="13312" width="22.140625" style="6"/>
+    <col min="13313" max="13313" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13316" max="13316" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13317" max="13317" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13318" max="13318" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13319" max="13319" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="16.85546875" style="6" customWidth="1"/>
+    <col min="13321" max="13321" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13322" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13323" max="13323" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13324" max="13324" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13325" max="13325" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13326" max="13326" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13327" width="27.7109375" style="6" customWidth="1"/>
+    <col min="13328" max="13338" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="13339" max="13345" width="20" style="6" customWidth="1"/>
+    <col min="13346" max="13346" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="13347" max="13347" width="22.140625" style="6" customWidth="1"/>
+    <col min="13348" max="13568" width="22.140625" style="6"/>
+    <col min="13569" max="13569" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13572" max="13572" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13573" max="13573" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13574" max="13574" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13575" max="13575" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="16.85546875" style="6" customWidth="1"/>
+    <col min="13577" max="13577" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13578" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13579" max="13579" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13580" max="13580" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13581" max="13581" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13582" max="13582" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13583" width="27.7109375" style="6" customWidth="1"/>
+    <col min="13584" max="13594" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="13595" max="13601" width="20" style="6" customWidth="1"/>
+    <col min="13602" max="13602" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="13603" max="13603" width="22.140625" style="6" customWidth="1"/>
+    <col min="13604" max="13824" width="22.140625" style="6"/>
+    <col min="13825" max="13825" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13828" max="13828" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="13829" max="13829" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13830" max="13830" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13831" max="13831" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="16.85546875" style="6" customWidth="1"/>
+    <col min="13833" max="13833" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13834" max="13834" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13835" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13836" max="13836" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13837" max="13837" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13838" max="13838" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="13839" max="13839" width="27.7109375" style="6" customWidth="1"/>
+    <col min="13840" max="13850" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="13851" max="13857" width="20" style="6" customWidth="1"/>
+    <col min="13858" max="13858" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="13859" max="13859" width="22.140625" style="6" customWidth="1"/>
+    <col min="13860" max="14080" width="22.140625" style="6"/>
+    <col min="14081" max="14081" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14084" max="14084" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14085" max="14085" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14086" max="14086" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14087" max="14087" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="16.85546875" style="6" customWidth="1"/>
+    <col min="14089" max="14089" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14090" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14091" max="14091" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14092" max="14092" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14093" max="14093" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14094" max="14094" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14095" width="27.7109375" style="6" customWidth="1"/>
+    <col min="14096" max="14106" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="14107" max="14113" width="20" style="6" customWidth="1"/>
+    <col min="14114" max="14114" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="14115" max="14115" width="22.140625" style="6" customWidth="1"/>
+    <col min="14116" max="14336" width="22.140625" style="6"/>
+    <col min="14337" max="14337" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14340" max="14340" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14341" max="14341" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14342" max="14342" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14343" max="14343" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="16.85546875" style="6" customWidth="1"/>
+    <col min="14345" max="14345" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14346" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14347" max="14347" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14348" max="14348" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14349" max="14349" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14350" max="14350" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14351" width="27.7109375" style="6" customWidth="1"/>
+    <col min="14352" max="14362" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="14363" max="14369" width="20" style="6" customWidth="1"/>
+    <col min="14370" max="14370" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="14371" max="14371" width="22.140625" style="6" customWidth="1"/>
+    <col min="14372" max="14592" width="22.140625" style="6"/>
+    <col min="14593" max="14593" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14596" max="14596" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14597" max="14597" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14598" max="14598" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14599" max="14599" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="16.85546875" style="6" customWidth="1"/>
+    <col min="14601" max="14601" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14602" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14603" max="14603" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14604" max="14604" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14605" max="14605" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14606" max="14606" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14607" width="27.7109375" style="6" customWidth="1"/>
+    <col min="14608" max="14618" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="14619" max="14625" width="20" style="6" customWidth="1"/>
+    <col min="14626" max="14626" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="14627" max="14627" width="22.140625" style="6" customWidth="1"/>
+    <col min="14628" max="14848" width="22.140625" style="6"/>
+    <col min="14849" max="14849" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14852" max="14852" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="14853" max="14853" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14854" max="14854" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14855" max="14855" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="16.85546875" style="6" customWidth="1"/>
+    <col min="14857" max="14857" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="14858" max="14858" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14859" max="14859" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14860" max="14860" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14861" max="14861" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14862" max="14862" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14863" max="14863" width="27.7109375" style="6" customWidth="1"/>
+    <col min="14864" max="14874" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="14875" max="14881" width="20" style="6" customWidth="1"/>
+    <col min="14882" max="14882" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="14883" max="14883" width="22.140625" style="6" customWidth="1"/>
+    <col min="14884" max="15104" width="22.140625" style="6"/>
+    <col min="15105" max="15105" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15108" max="15108" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15109" max="15109" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15110" max="15110" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15111" max="15111" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="16.85546875" style="6" customWidth="1"/>
+    <col min="15113" max="15113" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15114" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15115" max="15115" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15116" max="15116" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15117" max="15117" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15118" max="15118" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15119" width="27.7109375" style="6" customWidth="1"/>
+    <col min="15120" max="15130" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="15131" max="15137" width="20" style="6" customWidth="1"/>
+    <col min="15138" max="15138" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="15139" max="15139" width="22.140625" style="6" customWidth="1"/>
+    <col min="15140" max="15360" width="22.140625" style="6"/>
+    <col min="15361" max="15361" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15364" max="15364" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15365" max="15365" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15366" max="15366" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15367" max="15367" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="16.85546875" style="6" customWidth="1"/>
+    <col min="15369" max="15369" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15370" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15371" max="15371" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15372" max="15372" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15373" max="15373" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15374" max="15374" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15375" width="27.7109375" style="6" customWidth="1"/>
+    <col min="15376" max="15386" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="15387" max="15393" width="20" style="6" customWidth="1"/>
+    <col min="15394" max="15394" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="15395" max="15395" width="22.140625" style="6" customWidth="1"/>
+    <col min="15396" max="15616" width="22.140625" style="6"/>
+    <col min="15617" max="15617" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15620" max="15620" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15621" max="15621" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15622" max="15622" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15623" max="15623" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="16.85546875" style="6" customWidth="1"/>
+    <col min="15625" max="15625" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15626" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15627" max="15627" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15628" max="15628" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15629" max="15629" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15630" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15631" width="27.7109375" style="6" customWidth="1"/>
+    <col min="15632" max="15642" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="15643" max="15649" width="20" style="6" customWidth="1"/>
+    <col min="15650" max="15650" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="15651" max="15651" width="22.140625" style="6" customWidth="1"/>
+    <col min="15652" max="15872" width="22.140625" style="6"/>
+    <col min="15873" max="15873" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15876" max="15876" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15877" max="15877" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15878" max="15878" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15879" max="15879" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="16.85546875" style="6" customWidth="1"/>
+    <col min="15881" max="15881" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="15882" max="15882" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15883" max="15883" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15884" max="15884" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15885" max="15885" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="15886" max="15886" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="15887" max="15887" width="27.7109375" style="6" customWidth="1"/>
+    <col min="15888" max="15898" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="15899" max="15905" width="20" style="6" customWidth="1"/>
+    <col min="15906" max="15906" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="15907" max="15907" width="22.140625" style="6" customWidth="1"/>
+    <col min="15908" max="16128" width="22.140625" style="6"/>
+    <col min="16129" max="16129" width="7.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="4.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="19.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16132" max="16132" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="16133" max="16133" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16134" max="16134" width="12.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16135" max="16135" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="16.85546875" style="6" customWidth="1"/>
+    <col min="16137" max="16137" width="5.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16138" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16139" max="16139" width="8.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16140" max="16140" width="20.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16141" max="16141" width="20.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="16142" max="16142" width="27.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16143" width="27.7109375" style="6" customWidth="1"/>
+    <col min="16144" max="16154" width="20" style="6" bestFit="1" customWidth="1"/>
+    <col min="16155" max="16161" width="20" style="6" customWidth="1"/>
+    <col min="16162" max="16162" width="23" style="6" bestFit="1" customWidth="1"/>
+    <col min="16163" max="16163" width="22.140625" style="6" customWidth="1"/>
+    <col min="16164" max="16384" width="22.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+    </row>
+    <row r="2" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="10"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+    </row>
+    <row r="3" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="10"/>
+    </row>
+    <row r="4" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="J4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+      <c r="AF4" s="10"/>
+      <c r="AG4" s="10"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="6"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1"/>
   <sheetViews>
@@ -9026,13 +10516,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>29</v>
@@ -9053,7 +10543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -9071,16 +10561,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -9088,13 +10578,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="15">
         <v>500</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -9102,13 +10592,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="15">
         <v>1000</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -9116,13 +10606,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C4" s="15">
         <v>2000</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>